<commit_message>
CAN1-72 # Fixed issues in BTM_Test_Cases by Waseem
</commit_message>
<xml_diff>
--- a/Documentations/Test Cases/Bit_Timing_Module_Test_Cases.xlsx
+++ b/Documentations/Test Cases/Bit_Timing_Module_Test_Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Files\LTTS\FPGA Training\Projects\Verilog\Can_Controller\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{893C28E8-9F40-4C44-8CCD-BD82CE4F57EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C1A3A5-BB17-4D52-B0D2-3F1A2190B8D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1968" yWindow="2220" windowWidth="17280" windowHeight="10140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="192">
   <si>
     <t>Requirement Tag</t>
   </si>
@@ -573,117 +573,115 @@
     <t>int_ts2_next' is set to 'int_ts2' - 'i_sjw' when 'int_rx_prev' is not equal to 'int_rx_comp' and 'int_count' is less than 'int_ts1' - 'i_sjw'</t>
   </si>
   <si>
-    <t>1. 'int_rx_prev' != 'int_rx_comp'
-2. 'int_count' &lt; 'int_ts1' - 'i_sjw'</t>
-  </si>
-  <si>
-    <t>1. Wait until 'int_rx_prev' is not equal to 'int_rx_comp'
-2. Wait until 'int_count' is less than 'int_ts1' - 'i_sjw'
+    <t>int_ts2_next' = 'int_ts2' - 'i_sjw'</t>
+  </si>
+  <si>
+    <t>int_ts2_next' = 'int_ts2' - 'int_count'</t>
+  </si>
+  <si>
+    <t>int_ts1_next' is set to 'int_count' when 'int_rx_prev' is not equal to 'int_rx_comp' and 'int_count' is greater than or equal to 'int_ts1' and is less than 'int_ts1' + 'i_sjw'</t>
+  </si>
+  <si>
+    <t>int_ts2_next' is set to 'int_ts2' - 'int_count' when 'int_tx_prev' is not equal to 'int_rx_comp' and 'int_count' is less than 'int_ts1' and is greater than or equal to 'int_ts1' - 'i_sjw'</t>
+  </si>
+  <si>
+    <t>int_ts1_next' = 'int_count'</t>
+  </si>
+  <si>
+    <t>int_ts1_next' is set to 'int_ts1' + 'i_sjw' when 'int_rx_prev' is not equal to 'int_rx_comp' and 'int_count' is less than 'int_ts1' + 'i_sjw'</t>
+  </si>
+  <si>
+    <t>int_ts1_next' = 'int_ts1' + 'i_sjw'</t>
+  </si>
+  <si>
+    <t>int_ts1' is set to 'int_ts1_next' when 'int_state' is in SYNC state and 'int_rxbit_history'[5:0] is not equal to 6'b0 or 6'b111111</t>
+  </si>
+  <si>
+    <t>int_ts2' is set to 'i_ts2' + 1 when 'int_state' is in SYNC state and 'int_rxbit_history'[5:0] is equal to 6'b0 or 6'b111111</t>
+  </si>
+  <si>
+    <t>int_ts1' is set to 'i_ts1' + 1 when 'int_state' is in SYNC state and 'int_rxbit_history'[5:0] is equal to 6'b0 or 6'b111111</t>
+  </si>
+  <si>
+    <t>int_ts1' = 'int_ts1_next'</t>
+  </si>
+  <si>
+    <t>int_ts2' is set to 'int_ts2_next' when 'int_state' is in SYNC state and 'int_rxbit_history'[5:0] is not equal to 6'b0 or 6'b111111</t>
+  </si>
+  <si>
+    <t>int_ts2' = 'int_ts2_next'</t>
+  </si>
+  <si>
+    <t>int_rxbit_history'[5:0] is set to 'int_rxbit_history'[4:0] &amp; 'CAN_PHY_RX' when 'int_state' is set to SYNC state</t>
+  </si>
+  <si>
+    <t>int_rxbit_history'[5:0] = 'int_rxbit_history'[4:0] &amp; 'CAN_PHY_RX'</t>
+  </si>
+  <si>
+    <t>1. Wait until 'int_count' is less than 'int_ts1' - 'i_sjw'
+2. Set 'CAN_PHY_RX' to 1
 3. Check that 'int_ts2_next' is set to 'int_ts2' - 'i_sjw'</t>
   </si>
   <si>
-    <t>int_ts2_next' = 'int_ts2' - 'i_sjw'</t>
-  </si>
-  <si>
-    <t>1. 'int_rx_prev' != 'int_rx_comp'
-2. 'int_ts1' - 'i_sjw' &lt;= 'int_count' &lt; 'int_ts1'</t>
-  </si>
-  <si>
-    <t>1. Wait until 'int_rx_prev' is not equal to 'int_rx_comp'
-2. Wait until 'int_count' is less than 'int_ts1' and greater than or equal to 'int_ts1' - 'i_sjw'
+    <t>1. 'int_count' &lt; 'int_ts1' - 'i_sjw'
+2. 'CAN_PHY_RX' = 1</t>
+  </si>
+  <si>
+    <t>1. Wait until 'int_count' is less than 'int_ts1' and greater than or equal to 'int_ts1' - 'i_sjw'
+2. Set 'CAN_PHY_RX' to 0
 3. Check that 'int_ts2_next' is set to 'int_ts2' - 'int_count'</t>
   </si>
   <si>
-    <t>int_ts2_next' = 'int_ts2' - 'int_count'</t>
-  </si>
-  <si>
-    <t>int_ts1_next' is set to 'int_count' when 'int_rx_prev' is not equal to 'int_rx_comp' and 'int_count' is greater than or equal to 'int_ts1' and is less than 'int_ts1' + 'i_sjw'</t>
-  </si>
-  <si>
-    <t>int_ts2_next' is set to 'int_ts2' - 'int_count' when 'int_tx_prev' is not equal to 'int_rx_comp' and 'int_count' is less than 'int_ts1' and is greater than or equal to 'int_ts1' - 'i_sjw'</t>
-  </si>
-  <si>
-    <t>1. Wait until 'int_rx_prev' is not equal to 'int_rx_comp'
-2. wait until 'int_count' is greater than or equal to 'int_ts1' and less than 'int_ts1' + 'i_sjw'
+    <t>1. 'int_ts1' - 'i_sjw' &lt;= 'int_count' &lt; 'int_ts1'
+2. 'CAN_PHY_RX' = 0</t>
+  </si>
+  <si>
+    <t>1. Wait until 'int_count' is greater than or equal to 'int_ts1' and less than 'int_ts1' + 'i_sjw'
+2. Set 'CAN_PHY_RX' to 1
 3. Check that 'int_ts1_next' is set to 'int_count'</t>
   </si>
   <si>
-    <t>1. 'int_rx_prev' != 'int_rx_comp'
-2. 'int_ts1' &lt;= 'int_count' &lt; 'int_ts1' + 'i_sjw'</t>
-  </si>
-  <si>
-    <t>int_ts1_next' = 'int_count'</t>
-  </si>
-  <si>
-    <t>int_ts1_next' is set to 'int_ts1' + 'i_sjw' when 'int_rx_prev' is not equal to 'int_rx_comp' and 'int_count' is less than 'int_ts1' + 'i_sjw'</t>
-  </si>
-  <si>
-    <t>1. Wait until 'int_rx_prev' is not equal to 'int_rx_comp'
-2. Wait until 'int_count' is less than 'int_ts1' + 'i_sjw'
+    <t>1. 'int_ts1' &lt;= 'int_count' &lt; 'int_ts1' + 'i_sjw'
+2. 'CAN_PHY_RX' = 1</t>
+  </si>
+  <si>
+    <t>1. Wait until 'int_count' is less than 'int_ts1' + 'i_sjw'
+2. Set 'CAN_PHY_RX' to 0
 3. Check that 'int_ts1_next' is set to 'int_ts1' + 'i_sjw'</t>
   </si>
   <si>
-    <t>1. 'int_rx_prev' != 'int_rx_comp'
-2. 'int_count' &lt; 'int_ts1' + 'i_sjw'</t>
-  </si>
-  <si>
-    <t>int_ts1_next' = 'int_ts1' + 'i_sjw'</t>
-  </si>
-  <si>
-    <t>1. 'int_state' = SYNC
-2. 'int_rxbit_history' = 6'b0 | 'int_rxbit_history' = 6'b111111</t>
-  </si>
-  <si>
-    <t>1. Wait until 'int_state' is set to SYNC state
-2. Wait until 'int_rxbit_history'[5:0] is set to 6'b0 or 6'b111111
-3. Check that 'int_ts2' is set to 'i_ts2' + 1</t>
-  </si>
-  <si>
-    <t>1. Wait until 'int_state' is set to SYNC state
-2. Wait until 'int_rxbit_history'[5:0] is set to 6'b0 or 6'b111111
-3. Check that 'int_ts1' is set to 'i_ts1' + 1</t>
-  </si>
-  <si>
-    <t>int_ts1' is set to 'int_ts1_next' when 'int_state' is in SYNC state and 'int_rxbit_history'[5:0] is not equal to 6'b0 or 6'b111111</t>
-  </si>
-  <si>
-    <t>int_ts2' is set to 'i_ts2' + 1 when 'int_state' is in SYNC state and 'int_rxbit_history'[5:0] is equal to 6'b0 or 6'b111111</t>
-  </si>
-  <si>
-    <t>int_ts1' is set to 'i_ts1' + 1 when 'int_state' is in SYNC state and 'int_rxbit_history'[5:0] is equal to 6'b0 or 6'b111111</t>
+    <t>1. 'int_count' &lt; 'int_ts1' + 'i_sjw'
+2. 'CAN_PHY_RX' = 0</t>
+  </si>
+  <si>
+    <t>1. Wait until 'int_rxbit_history'[5:0] is set to 6'b0 or 6'b111111
+2. Wait until 'int_state' is set to SYNC state
+3. Check that 'int_ts1' is set to 'i_ts1' + 1
+4. Check that 'int_ts2' is set to 'i_ts2' + 1</t>
   </si>
   <si>
     <t>1. Wait until 'int_state' is set to SYNC state
 2. Wait until 'int_rxbit_history'[5:0] is not equal to 6'b0 or 6'b111111
-3. Check that 'int_ts1' is set to 'int_ts1_next'</t>
-  </si>
-  <si>
-    <t>1. 'int_state' = SYNC
-2. 'int_rxbit_history' != 6'b0 &amp; 'int_rxbit_history' != 6'b111111</t>
-  </si>
-  <si>
-    <t>int_ts1' = 'int_ts1_next'</t>
-  </si>
-  <si>
-    <t>int_ts2' is set to 'int_ts2_next' when 'int_state' is in SYNC state and 'int_rxbit_history'[5:0] is not equal to 6'b0 or 6'b111111</t>
-  </si>
-  <si>
-    <t>1. Wait until 'int_state' is set to SYNC state
-2. Wait until 'int_rxbit_history'[5:0] is not equal to 6'b0 or 6'b111111
-3. Check that 'int_ts2' is set to 'int_ts2_next'</t>
-  </si>
-  <si>
-    <t>int_ts2' = 'int_ts2_next'</t>
-  </si>
-  <si>
-    <t>int_rxbit_history'[5:0] is set to 'int_rxbit_history'[4:0] &amp; 'CAN_PHY_RX' when 'int_state' is set to SYNC state</t>
-  </si>
-  <si>
-    <t>1. Wait until 'int_state' is set to SYNC state
-2. Check that 'int_rxbit_history'[5:0] is set to 'int_rxbit_history'[4:0] &amp; 'CAN_PHY_RX'</t>
-  </si>
-  <si>
-    <t>int_rxbit_history'[5:0] = 'int_rxbit_history'[4:0] &amp; 'CAN_PHY_RX'</t>
+3. Check that 'int_ts1' is set to 'int_ts1_next'
+4. Check that 'int_ts2' is set to 'int_ts2_next'</t>
+  </si>
+  <si>
+    <t>1. 'CAN_PHY_RX' = 0 for 6 bit times
+2. 'int_state' = SYNC
+3. 'int_rxbit_history' = 6'b0 | 'int_rxbit_history' = 6'b111111</t>
+  </si>
+  <si>
+    <t>1. 'CAN_PHY_RX' = 0 for 6 bit times
+2. 'int_state' = SYNC
+3. 'int_rxbit_history' != 6'b0 &amp; 'int_rxbit_history' != 6'b111111</t>
+  </si>
+  <si>
+    <t>1. Set 'CAN_PHY_RX' to 1
+2. Wait until 'int_state' is set to SYNC state
+3. Check that 'int_rxbit_history'[5:0] is set to 'int_rxbit_history'[4:0] &amp; 'CAN_PHY_RX'
+4. Set 'CAN_PHY_RX' to 0
+5. Wait until 'int_state' is set to SYNC state
+6. Check that 'int_rxbit_history'[5:0] is set to 'int_rxbit_history'[4:0] &amp; 'CAN_PHY_RX'</t>
   </si>
 </sst>
 </file>
@@ -733,7 +731,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -746,6 +744,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1063,8 +1064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C30" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1661,7 +1662,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>36</v>
       </c>
@@ -1672,16 +1673,16 @@
         <v>163</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
       <c r="E28" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="F28" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="F28" s="6" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>37</v>
       </c>
@@ -1689,19 +1690,19 @@
         <v>72</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>167</v>
+        <v>182</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>38</v>
       </c>
@@ -1709,19 +1710,19 @@
         <v>73</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>39</v>
       </c>
@@ -1729,19 +1730,19 @@
         <v>74</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>40</v>
       </c>
@@ -1749,19 +1750,19 @@
         <v>75</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>179</v>
+        <v>173</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>189</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>41</v>
       </c>
@@ -1769,19 +1770,15 @@
         <v>76</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>179</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
       <c r="F33" s="6" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>42</v>
       </c>
@@ -1789,19 +1786,19 @@
         <v>77</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>186</v>
+        <v>171</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>190</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>43</v>
       </c>
@@ -1809,19 +1806,15 @@
         <v>78</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>186</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
       <c r="F35" s="6" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>44</v>
       </c>
@@ -1829,19 +1822,25 @@
         <v>79</v>
       </c>
       <c r="C36" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>192</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>122</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1849,21 +1848,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010008B8F660E2FD5A4F9C25F557691C2E7B" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="291a90324d5b7e405cdee1cca19d0e54">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0fe6e073-fbcf-4c9f-9467-c4294a786ad2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1a3d94df2e09d7482e07420c2cba8fd2" ns2:_="">
     <xsd:import namespace="0fe6e073-fbcf-4c9f-9467-c4294a786ad2"/>
@@ -2009,24 +1993,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA12D9B4-0AFF-4A48-8503-C4B7A72BF3AD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{065C203B-187E-495A-97A5-35B3AD3DB734}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{099A5288-121E-4A14-A6B4-83046D76B9FD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2042,4 +2024,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{065C203B-187E-495A-97A5-35B3AD3DB734}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA12D9B4-0AFF-4A48-8503-C4B7A72BF3AD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
CAN1-74 # BTM_Test_Cases by Waseem
</commit_message>
<xml_diff>
--- a/Documentations/Test Cases/Bit_Timing_Module_Test_Cases.xlsx
+++ b/Documentations/Test Cases/Bit_Timing_Module_Test_Cases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Files\LTTS\FPGA Training\Projects\Verilog\Can_Controller\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Files\LTTS\FPGA Training\Projects\Verilog\Can_Controller\git_repo\Documentations\Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C1A3A5-BB17-4D52-B0D2-3F1A2190B8D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DDEF4C5-7A06-4A3A-8A04-C950764C299E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -660,20 +660,9 @@
 4. Check that 'int_ts2' is set to 'i_ts2' + 1</t>
   </si>
   <si>
-    <t>1. Wait until 'int_state' is set to SYNC state
-2. Wait until 'int_rxbit_history'[5:0] is not equal to 6'b0 or 6'b111111
-3. Check that 'int_ts1' is set to 'int_ts1_next'
-4. Check that 'int_ts2' is set to 'int_ts2_next'</t>
-  </si>
-  <si>
     <t>1. 'CAN_PHY_RX' = 0 for 6 bit times
 2. 'int_state' = SYNC
 3. 'int_rxbit_history' = 6'b0 | 'int_rxbit_history' = 6'b111111</t>
-  </si>
-  <si>
-    <t>1. 'CAN_PHY_RX' = 0 for 6 bit times
-2. 'int_state' = SYNC
-3. 'int_rxbit_history' != 6'b0 &amp; 'int_rxbit_history' != 6'b111111</t>
   </si>
   <si>
     <t>1. Set 'CAN_PHY_RX' to 1
@@ -682,6 +671,20 @@
 4. Set 'CAN_PHY_RX' to 0
 5. Wait until 'int_state' is set to SYNC state
 6. Check that 'int_rxbit_history'[5:0] is set to 'int_rxbit_history'[4:0] &amp; 'CAN_PHY_RX'</t>
+  </si>
+  <si>
+    <t>1. 'CAN_PHY_RX' = 0 for 3 bit times
+2. 'CAN_PHY_RX' = 1 for 3 bit times
+3. 'int_state' = SYNC
+4. 'int_rxbit_history' != 6'b0 &amp; 'int_rxbit_history' != 6'b111111</t>
+  </si>
+  <si>
+    <t>1. Wait for 3 bit times
+2. Set 'CAN_PHY_RX' to 1
+3. Wait until 'int_rxbit_history'[5:0] is not equal to 6'b0 or 6'b111111
+4. Wait until 'int_state' is set to SYNC state
+5. Check that 'int_ts1' is set to 'int_ts1_next'
+6. Check that 'int_ts2' is set to 'int_ts2_next'</t>
   </si>
 </sst>
 </file>
@@ -1065,7 +1068,7 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+      <selection activeCell="E34" sqref="E34:E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1756,7 +1759,7 @@
         <v>187</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>114</v>
@@ -1789,7 +1792,7 @@
         <v>171</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>190</v>
@@ -1825,7 +1828,7 @@
         <v>177</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>122</v>
@@ -1848,6 +1851,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010008B8F660E2FD5A4F9C25F557691C2E7B" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="291a90324d5b7e405cdee1cca19d0e54">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0fe6e073-fbcf-4c9f-9467-c4294a786ad2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1a3d94df2e09d7482e07420c2cba8fd2" ns2:_="">
     <xsd:import namespace="0fe6e073-fbcf-4c9f-9467-c4294a786ad2"/>
@@ -1993,22 +2011,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA12D9B4-0AFF-4A48-8503-C4B7A72BF3AD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{065C203B-187E-495A-97A5-35B3AD3DB734}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{099A5288-121E-4A14-A6B4-83046D76B9FD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2024,21 +2044,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{065C203B-187E-495A-97A5-35B3AD3DB734}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA12D9B4-0AFF-4A48-8503-C4B7A72BF3AD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>